<commit_message>
mudanca em nome de variáveis
</commit_message>
<xml_diff>
--- a/data/func_log.xlsx
+++ b/data/func_log.xlsx
@@ -521,8 +521,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -534,8 +536,10 @@
           <t>FINANÇAS</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>12345678910</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12345678910</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -552,8 +556,10 @@
           <t>MARIA SILVA</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>123</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
@@ -571,17 +577,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M2" t="n">
-        <v>12345678</v>
-      </c>
-      <c r="N2" t="n">
-        <v>83</v>
-      </c>
-      <c r="O2" t="n">
-        <v>987654321</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>987654321</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -590,8 +604,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -603,8 +619,10 @@
           <t>ATENDIMENTO</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>12225442972</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>12225442972</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -613,24 +631,34 @@
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
-        <v>0</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -639,8 +667,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -652,8 +682,10 @@
           <t>TECNOLOGIA</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>98765432198</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>98765432198</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -662,24 +694,34 @@
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>0</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -688,8 +730,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -701,8 +745,10 @@
           <t>MARKETING</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>73270102760</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>73270102760</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -719,8 +765,10 @@
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>1011</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1011</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
@@ -738,17 +786,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M5" t="n">
-        <v>34567890</v>
-      </c>
-      <c r="N5" t="n">
-        <v>83</v>
-      </c>
-      <c r="O5" t="n">
-        <v>987654321</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>34567890</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>987654321</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -757,8 +813,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -770,30 +828,42 @@
           <t>ATENDIMENTO</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>87617978563</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>87617978563</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
-        <v>0</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>83</v>
-      </c>
-      <c r="O6" t="n">
-        <v>987654321</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>987654321</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -802,8 +872,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -815,8 +887,10 @@
           <t>MARKETING</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>96912552852</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>96912552852</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -829,8 +903,10 @@
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
@@ -848,17 +924,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M7" t="n">
-        <v>53233133</v>
-      </c>
-      <c r="N7" t="n">
-        <v>83</v>
-      </c>
-      <c r="O7" t="n">
-        <v>902641692</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>53233133</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>902641692</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -867,8 +951,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -880,8 +966,10 @@
           <t>SUPORTE TÉCNICO</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>65075493546</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>65075493546</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -898,8 +986,10 @@
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>1617</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1617</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
@@ -917,17 +1007,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M8" t="n">
-        <v>65976313</v>
-      </c>
-      <c r="N8" t="n">
-        <v>83</v>
-      </c>
-      <c r="O8" t="n">
-        <v>986992168</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>65976313</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>986992168</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -936,8 +1034,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -949,8 +1049,10 @@
           <t>RECURSOS HUMANOS</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>45678912365</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>45678912365</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -967,8 +1069,10 @@
           <t>JULIANA SOUZA</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>456</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
@@ -986,17 +1090,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M9" t="n">
-        <v>65432109</v>
-      </c>
-      <c r="N9" t="n">
-        <v>83</v>
-      </c>
-      <c r="O9" t="n">
-        <v>987654321</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>65432109</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>987654321</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1005,8 +1117,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1018,8 +1132,10 @@
           <t>MARKETING</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>85296374100</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>85296374100</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1028,8 +1144,10 @@
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="n">
-        <v>0</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
@@ -1047,17 +1165,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M10" t="n">
-        <v>32109876</v>
-      </c>
-      <c r="N10" t="n">
-        <v>83</v>
-      </c>
-      <c r="O10" t="n">
-        <v>987654321</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>32109876</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>987654321</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1066,8 +1192,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1079,8 +1207,10 @@
           <t>PESQUISA</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>75138852164</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>75138852164</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
@@ -1089,8 +1219,10 @@
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="n">
-        <v>0</v>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
@@ -1108,17 +1240,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M11" t="n">
-        <v>59799845</v>
-      </c>
-      <c r="N11" t="n">
-        <v>83</v>
-      </c>
-      <c r="O11" t="n">
-        <v>998858160</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>59799845</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>998858160</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1127,8 +1267,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1140,8 +1282,10 @@
           <t>RECURSOS HUMANOS</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>50977808264</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>50977808264</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -1150,8 +1294,10 @@
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H12" t="n">
-        <v>0</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
@@ -1165,17 +1311,25 @@
           <t>PB</t>
         </is>
       </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>83</v>
-      </c>
-      <c r="O12" t="n">
-        <v>916221063</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>916221063</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1184,8 +1338,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1197,8 +1353,10 @@
           <t>SUPORTE TÉCNICO</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>36985214700</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>36985214700</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1215,24 +1373,34 @@
           <t>CAROLINA COSTA</t>
         </is>
       </c>
-      <c r="H13" t="n">
-        <v>0</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1241,8 +1409,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1254,8 +1424,10 @@
           <t>ATENDIMENTO</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>14725836900</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>14725836900</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1272,24 +1444,34 @@
           <t>MARIA LIMA</t>
         </is>
       </c>
-      <c r="H14" t="n">
-        <v>0</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -1298,8 +1480,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1311,8 +1495,10 @@
           <t>RECURSOS HUMANOS</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>51147045250</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>51147045250</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
@@ -1325,24 +1511,34 @@
           <t>JULIA FERNANDES</t>
         </is>
       </c>
-      <c r="H15" t="n">
-        <v>0</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>83</v>
-      </c>
-      <c r="O15" t="n">
-        <v>931857921</v>
-      </c>
-      <c r="P15" t="n">
-        <v>0</v>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>931857921</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>

</xml_diff>